<commit_message>
changes into the script
</commit_message>
<xml_diff>
--- a/real_data/resnet101_CIFAR.xlsx
+++ b/real_data/resnet101_CIFAR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joanatirana/Desktop/delft-visiting/optimize code/scheduling-jobs/real_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C7C8FB-85DF-3744-BEDB-7D3D0A4C7D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1920F2-A1FB-3D4B-BB90-187505717FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25600" yWindow="6100" windowWidth="25600" windowHeight="15500" activeTab="5" xr2:uid="{7935258D-7BA1-BE4D-B533-9C0418764F7B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="6" xr2:uid="{7935258D-7BA1-BE4D-B533-9C0418764F7B}"/>
   </bookViews>
   <sheets>
     <sheet name="VM" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -56,6 +56,13 @@
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -78,9 +85,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,15 +403,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3907375A-5822-0A45-92DF-EC04FBC81381}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>3.2307700000000001</v>
       </c>
@@ -414,7 +422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>3.30769</v>
       </c>
@@ -425,7 +433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>6.61538</v>
       </c>
@@ -436,7 +444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>6.61538</v>
       </c>
@@ -447,7 +455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>6.5384599999999997</v>
       </c>
@@ -458,7 +466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>7.61538</v>
       </c>
@@ -468,8 +476,10 @@
       <c r="C6" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6.61538</v>
       </c>
@@ -479,12 +489,10 @@
       <c r="C7" s="1">
         <v>0</v>
       </c>
-      <c r="F7">
-        <f>SUM(A6:A33)</f>
-        <v>252.53844000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6.61538</v>
       </c>
@@ -495,7 +503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>6.61538</v>
       </c>
@@ -506,7 +514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>10.0769</v>
       </c>
@@ -517,7 +525,7 @@
         <v>1.0769200000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>8.7692300000000003</v>
       </c>
@@ -528,7 +536,7 @@
         <v>1.0769200000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>8.7692300000000003</v>
       </c>
@@ -539,7 +547,7 @@
         <v>1.0769200000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>8.7692300000000003</v>
       </c>
@@ -550,7 +558,7 @@
         <v>1.0769200000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>8.7692300000000003</v>
       </c>
@@ -561,7 +569,7 @@
         <v>1.0769200000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>8.6923100000000009</v>
       </c>
@@ -572,7 +580,7 @@
         <v>1.0769200000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>8.9230800000000006</v>
       </c>
@@ -821,15 +829,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF728E79-D3DB-1040-8D51-06514020BC7B}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>34.153799999999997</v>
       </c>
@@ -840,7 +848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>3.2307700000000001</v>
       </c>
@@ -851,7 +859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>13.307700000000001</v>
       </c>
@@ -862,7 +870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>13.2308</v>
       </c>
@@ -873,7 +881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>13.461499999999999</v>
       </c>
@@ -884,7 +892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>77.230800000000002</v>
       </c>
@@ -894,12 +902,8 @@
       <c r="C6">
         <v>0</v>
       </c>
-      <c r="F6">
-        <f>SUM(A6:A33)</f>
-        <v>1810.30827</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>7.7692300000000003</v>
       </c>
@@ -910,7 +914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7.5384599999999997</v>
       </c>
@@ -921,7 +925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7.9230799999999997</v>
       </c>
@@ -932,7 +936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>239.46199999999999</v>
       </c>
@@ -943,7 +947,7 @@
         <v>0.34426200000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>20.461500000000001</v>
       </c>
@@ -954,7 +958,7 @@
         <v>8.1967200000000004E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>20</v>
       </c>
@@ -965,7 +969,7 @@
         <v>6.5573800000000002E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>19.8462</v>
       </c>
@@ -976,7 +980,7 @@
         <v>0.163934</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>20</v>
       </c>
@@ -987,7 +991,7 @@
         <v>0.13114799999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>20.230799999999999</v>
       </c>
@@ -998,7 +1002,7 @@
         <v>0.18032799999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>20</v>
       </c>
@@ -1249,7 +1253,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F3ECEB3-F06F-004D-B5F3-5A36A880D2D3}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1670,17 +1676,17 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
-        <v>0</v>
+        <v>269</v>
       </c>
       <c r="B1" s="1">
-        <v>0</v>
+        <v>124</v>
       </c>
       <c r="C1" s="1">
         <v>0</v>
@@ -1688,10 +1694,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>0</v>
+        <v>55.461500000000001</v>
       </c>
       <c r="B2" s="1">
-        <v>0</v>
+        <v>79.615399999999994</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
@@ -2514,8 +2520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA781742-6964-264E-BD04-C0478125399C}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2936,8 +2942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DB2EFC7-8096-8542-AF66-11F811B1415F}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A41" sqref="A38:A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
adding readme file for the profiled data
</commit_message>
<xml_diff>
--- a/real_data/resnet101_CIFAR.xlsx
+++ b/real_data/resnet101_CIFAR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joanatirana/Documents/research/delft-visiting/optimize code/scheduling-jobs/real_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joanatirana/Documents/coding/git_repos/SFL-workflow-optimization/real_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61BC019D-1376-164D-A8E9-FAB0EE233785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0078ED-C180-1F4F-BD3A-5CE0F38183B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{7935258D-7BA1-BE4D-B533-9C0418764F7B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="6" xr2:uid="{7935258D-7BA1-BE4D-B533-9C0418764F7B}"/>
   </bookViews>
   <sheets>
     <sheet name="VM" sheetId="1" r:id="rId1"/>
@@ -405,7 +405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3907375A-5822-0A45-92DF-EC04FBC81381}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
@@ -2945,15 +2945,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DB2EFC7-8096-8542-AF66-11F811B1415F}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>8193.568359375</v>
       </c>
@@ -2961,7 +2961,7 @@
         <v>39.435546875</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>2049.568359375</v>
       </c>
@@ -2969,7 +2969,7 @@
         <v>5.353515625</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2049.568359375</v>
       </c>
@@ -2977,7 +2977,7 @@
         <v>298.00390625</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2049.568359375</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>298.00390625</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>2049.568359375</v>
       </c>
@@ -2993,7 +2993,7 @@
         <v>298.00390625</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>1025.568359375</v>
       </c>
@@ -3001,7 +3001,7 @@
         <v>1169.599609375</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>1025.568359375</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>1164.00390625</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>1025.568359375</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>1164.00390625</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>1025.568359375</v>
       </c>
@@ -3025,7 +3025,7 @@
         <v>1164.00390625</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>513.568359375</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>4631.599609375</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>513.568359375</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>4624.00390625</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>513.568359375</v>
       </c>
@@ -3049,7 +3049,7 @@
         <v>4624.00390625</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>513.568359375</v>
       </c>
@@ -3057,31 +3057,23 @@
         <v>4624.00390625</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>513.568359375</v>
       </c>
       <c r="B14" s="1">
         <v>4624.00390625</v>
       </c>
-      <c r="D14">
-        <f>SUM(A18:B33)/1024</f>
-        <v>93.543703079223633</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>513.568359375</v>
       </c>
       <c r="B15" s="1">
         <v>4624.00390625</v>
       </c>
-      <c r="D15">
-        <f>SUM(A10:B34)/1024</f>
-        <v>151.96337699890137</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>513.568359375</v>
       </c>

</xml_diff>